<commit_message>
Continue modiffying OD class interface.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -634,8 +634,8 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modify method to calculate eac of track.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mob" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>turnout_freq</t>
   </si>
@@ -204,12 +204,6 @@
     <t>coef_b_track_cost</t>
   </si>
   <si>
-    <t>crf_track</t>
-  </si>
-  <si>
-    <t>Capital recovery factor of the track.</t>
-  </si>
-  <si>
     <t>Coefficient "b" for track maintenance cost equation (coef).</t>
   </si>
   <si>
@@ -240,9 +234,6 @@
     <t>Weight of a locomotive (ton).</t>
   </si>
   <si>
-    <t>Wage cost of maintaining a turnout.</t>
-  </si>
-  <si>
     <t>yearly_wages_by_turnout</t>
   </si>
   <si>
@@ -256,6 +247,33 @@
   </si>
   <si>
     <t>Minimum density to consider a link as being a main track (ton-km/ton = ton).</t>
+  </si>
+  <si>
+    <t>gross_tk_in_hq_track_lifetime</t>
+  </si>
+  <si>
+    <t>high_quality_track_price</t>
+  </si>
+  <si>
+    <t>interest_rate</t>
+  </si>
+  <si>
+    <t>Interest rate used to calculate capital recovery factor (rate).</t>
+  </si>
+  <si>
+    <t>Wage cost of maintaining a turnout (USD).</t>
+  </si>
+  <si>
+    <t>Design tons for high quality track. Gross tons that a hq track is suposed to support during its lifetime (gross ton-km).</t>
+  </si>
+  <si>
+    <t>The price of 1km of hight quality track (USD/km).</t>
+  </si>
+  <si>
+    <t>max_path_difference</t>
+  </si>
+  <si>
+    <t>Maximum difference in paths distance between rail and road options (coeff). Derivation won't happen if rail path is much longer than road path.</t>
   </si>
 </sst>
 </file>
@@ -634,7 +652,7 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -864,46 +882,46 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="4">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="4">
         <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B23" s="4">
         <v>1.67</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B24" s="5">
         <v>760000</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -917,16 +935,16 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="92" customWidth="1"/>
   </cols>
   <sheetData>
@@ -971,7 +989,7 @@
         <v>10.34046</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -993,7 +1011,7 @@
         <v>458.46100000000001</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1004,7 +1022,7 @@
         <v>175000</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,40 +1033,62 @@
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B9" s="4">
-        <v>8.8827433387272267E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4">
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" s="5">
         <v>109500</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="5">
+        <v>200000000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="5">
+        <v>800000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1061,10 +1101,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,6 +1179,17 @@
         <v>52</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rework classes to add different treatment to each product category. Derivation and regrouping rules are now different for each product category.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="mob" sheetId="1" r:id="rId1"/>
-    <sheet name="inf" sheetId="2" r:id="rId2"/>
-    <sheet name="deriv" sheetId="3" r:id="rId3"/>
+    <sheet name="mobility" sheetId="1" r:id="rId1"/>
+    <sheet name="infrastructure" sheetId="2" r:id="rId2"/>
+    <sheet name="derivation" sheetId="3" r:id="rId3"/>
+    <sheet name="categories" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">mob!$A$1:$C$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">mobility!$A$1:$C$20</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="107">
   <si>
     <t>turnout_freq</t>
   </si>
@@ -280,6 +281,66 @@
   </si>
   <si>
     <t>Maximum distance density (gross ton) supported by maximum distance turnouts (ton). Above this density, more turnouts are needed (distance between them is less).</t>
+  </si>
+  <si>
+    <t>max_derivation_1</t>
+  </si>
+  <si>
+    <t>max_derivation_2</t>
+  </si>
+  <si>
+    <t>max_derivation_3</t>
+  </si>
+  <si>
+    <t>max_derivation_4</t>
+  </si>
+  <si>
+    <t>max_derivation_5</t>
+  </si>
+  <si>
+    <t>regroup_1</t>
+  </si>
+  <si>
+    <t>regroup_2</t>
+  </si>
+  <si>
+    <t>regroup_3</t>
+  </si>
+  <si>
+    <t>regroup_4</t>
+  </si>
+  <si>
+    <t>regroup_5</t>
+  </si>
+  <si>
+    <t>Maximum % of derivation for product category 1 - grains (coeff).</t>
+  </si>
+  <si>
+    <t>Maximum % of derivation for product category 2 - primary products no grains (coeff).</t>
+  </si>
+  <si>
+    <t>Maximum % of derivation for product category 3 - semi manufactured (coeff).</t>
+  </si>
+  <si>
+    <t>Maximum % of derivation for product category 4 - manufactured (coeff).</t>
+  </si>
+  <si>
+    <t>Maximum % of derivation for product category 5 - unknown (coeff).</t>
+  </si>
+  <si>
+    <t>Regroup trains to reduce idle capacity (1=yes, 0=no) for product category 1 - grains (coeff).</t>
+  </si>
+  <si>
+    <t>Regroup trains to reduce idle capacity (1=yes, 0=no) for product category 2 - primary products no grains (coeff).</t>
+  </si>
+  <si>
+    <t>Regroup trains to reduce idle capacity (1=yes, 0=no) for product category 3 - semi manufactured (coeff).</t>
+  </si>
+  <si>
+    <t>Regroup trains to reduce idle capacity (1=yes, 0=no) for product category 4 - manufactured (coeff).</t>
+  </si>
+  <si>
+    <t>Regroup trains to reduce idle capacity (1=yes, 0=no) for product category 5 - unknown (coeff).</t>
   </si>
 </sst>
 </file>
@@ -658,8 +719,8 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,7 +1182,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1210,4 +1271,148 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="107.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2">
+        <v>0.8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3">
+        <v>0.7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4">
+        <v>0.7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rework report methods and classes to allow appending reports into the same excel, rather than generating new files for each report. Also clean up some other things.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -720,7 +720,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="4">
-        <v>3</v>
+        <v>0.01</v>
       </c>
       <c r="C20" t="s">
         <v>49</v>
@@ -1281,7 +1281,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Create unit test for modal_networks module and rework railway_cost for track cost methods. Modify classes in modal_networks module to be more testable by allowing to pass a builder.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -719,8 +719,8 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1280,7 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Complete first simple RoadwayNetwork class. Rework report, and cost modules to support methods of RoadwayNetwork. Change names of modules and imports to reflect new road classes.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -76,12 +76,6 @@
     <t>Time a train is parked at origin or destination (hr).</t>
   </si>
   <si>
-    <t>Loading capacity of a wagon (ton).</t>
-  </si>
-  <si>
-    <t>Towing capacity of a locomotive (ton).</t>
-  </si>
-  <si>
     <t>Time in a year a wagon is available to be used (hr/year).</t>
   </si>
   <si>
@@ -341,6 +335,12 @@
   </si>
   <si>
     <t>Regroup trains to reduce idle capacity (1=yes, 0=no) for product category 5 - unknown (coeff).</t>
+  </si>
+  <si>
+    <t>Towing capacity of a locomotive (ton). - Using 0,56 loading factor to account for empty returning locomotives.</t>
+  </si>
+  <si>
+    <t>Loading capacity of a wagon (ton). - Using 0,56 loading factor to account for empty returning wagons.</t>
   </si>
 </sst>
 </file>
@@ -720,7 +720,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +765,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>15</v>
@@ -776,13 +776,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3">
         <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>33.6</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,7 +804,7 @@
         <v>1276.8000000000002</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
         <v>8672</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,7 +826,7 @@
         <v>6570</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -834,7 +834,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
         <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -856,139 +856,139 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5">
         <v>6463.835901091652</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="5">
         <v>154445.87620922364</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="4">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="9">
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5">
         <v>100170</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="5">
         <v>2487.6562500000005</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="7">
         <v>30.416666666666668</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4">
         <v>0.01</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" s="4">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="4">
         <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="4">
         <v>1.67</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" s="5">
         <v>700000</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1005,7 +1005,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,123 +1028,123 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4">
         <v>-0.62124999999999997</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" s="4">
         <v>10.34046</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4">
         <v>-0.93081999999999998</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="4">
         <v>458.46100000000001</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4">
         <v>175000</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4">
         <v>3.1250000000000002E-3</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B8" s="4">
         <v>0.08</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4">
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B10" s="5">
         <v>109500</v>
       </c>
       <c r="C10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B11" s="5">
         <v>200000000</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="5">
         <v>800000</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,18 +1155,18 @@
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="5">
         <v>1200000</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1210,7 +1210,7 @@
         <v>5000</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1221,51 +1221,51 @@
         <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="8">
         <v>0.8</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4">
         <v>500</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="5">
         <v>120000</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" s="4">
         <v>0.5</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1304,112 +1304,112 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2">
         <v>0.8</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4">
         <v>0.7</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5">
         <v>0.6</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6">
         <v>0.5</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement several derivation methods on FreightNetwork class. Minor rework on modal_networks and report module.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -720,7 +720,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +985,7 @@
         <v>71</v>
       </c>
       <c r="B24" s="5">
-        <v>700000</v>
+        <v>750000</v>
       </c>
       <c r="C24" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Fix bug when creating empty od pairs. Add safeguards to prevent empty od pairs. Prevent several "division by zero" errors. Rework docstrings of future methods of FregithNetwork class.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -720,7 +720,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="4">
-        <v>0.01</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
@@ -985,7 +985,7 @@
         <v>71</v>
       </c>
       <c r="B24" s="5">
-        <v>750000</v>
+        <v>700000</v>
       </c>
       <c r="C24" t="s">
         <v>72</v>
@@ -1005,7 +1005,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,7 +1281,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rework test_cost to make work ok simplified way of testing. Start to add methods to costs related to time in RailwayNetworkCost module, they still doesn't work. Needs to be implemented and client classes reworked to use them.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
     <sheet name="infrastructure" sheetId="2" r:id="rId2"/>
-    <sheet name="derivation" sheetId="3" r:id="rId3"/>
-    <sheet name="categories" sheetId="4" r:id="rId4"/>
+    <sheet name="time" sheetId="5" r:id="rId3"/>
+    <sheet name="derivation" sheetId="3" r:id="rId4"/>
+    <sheet name="categories" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">mobility!$A$1:$C$20</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
   <si>
     <t>turnout_freq</t>
   </si>
@@ -341,6 +342,30 @@
   </si>
   <si>
     <t>Loading capacity of a wagon (ton). - Using 0,56 loading factor to account for empty returning wagons.</t>
+  </si>
+  <si>
+    <t>deposit_cost_per_day_ton</t>
+  </si>
+  <si>
+    <t>Cost of hold a ton of freight in a deposit one day (USD/ton-day).</t>
+  </si>
+  <si>
+    <t>ratio_truck_to_train_travel_time</t>
+  </si>
+  <si>
+    <t>Ratio of truck travel time to train travel time (coeff). Truck is always faster than train.</t>
+  </si>
+  <si>
+    <t>cost_of_immobilized_ton</t>
+  </si>
+  <si>
+    <t>Its the opportunity cost of having value immobilized over time, calculated as day interest rate * average freight value of a ton (USD/ton-day).</t>
+  </si>
+  <si>
+    <t>short_freight_to_train</t>
+  </si>
+  <si>
+    <t>Average cost of transport from door to train station (USD/ton).</t>
   </si>
 </sst>
 </file>
@@ -719,8 +744,8 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,10 +1204,88 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="92.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2">
+        <v>0.11853075454128587</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <v>1.1752104423052856</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>

</xml_diff>

<commit_message>
Rework tests for new objects structure in cost module. Rework OD to store costs results of the od pair.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
   <si>
     <t>turnout_freq</t>
   </si>
@@ -366,6 +366,18 @@
   </si>
   <si>
     <t>Average cost of transport from door to train station (USD/ton).</t>
+  </si>
+  <si>
+    <t>loading_ratio</t>
+  </si>
+  <si>
+    <t>Ratio of average net loading over total capacity per train or wagon (coeff). It reflects empty trains coming back to origin after doing a service.</t>
+  </si>
+  <si>
+    <t>min_weekly_freq</t>
+  </si>
+  <si>
+    <t>Minimum trains per week that have to be to service an od pair (number).</t>
   </si>
 </sst>
 </file>
@@ -742,10 +754,10 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,6 +1026,28 @@
       </c>
       <c r="C24" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1029,9 +1063,7 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1206,8 +1238,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1416,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Complete modifications to report new costs.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -754,10 +754,10 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,17 +1037,6 @@
       </c>
       <c r="C25" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="4">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1236,10 +1225,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,6 +1291,17 @@
       </c>
       <c r="C5" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rework classes to keep track of freight characteristics (category, original transport mode and od pair) at the level of links. Tons management at links has been removed out of Link class to a Tons superclass.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -756,8 +756,8 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1022,7 @@
         <v>71</v>
       </c>
       <c r="B24" s="5">
-        <v>700000</v>
+        <v>100000</v>
       </c>
       <c r="C24" t="s">
         <v>72</v>
@@ -1227,7 +1227,7 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rework way of determining if a link is a main track. Keep track of this characteristic on links properties to later report it.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -239,9 +239,6 @@
     <t>main_min_density</t>
   </si>
   <si>
-    <t>Minimum density to consider a link as being a main track (ton-km/ton = ton).</t>
-  </si>
-  <si>
     <t>gross_tk_in_hq_track_lifetime</t>
   </si>
   <si>
@@ -378,6 +375,9 @@
   </si>
   <si>
     <t>Minimum trains per week that have to be to service an od pair (number).</t>
+  </si>
+  <si>
+    <t>Minimum net density to consider a link as being a main track (ton-km/ton = ton).</t>
   </si>
 </sst>
 </file>
@@ -830,7 +830,7 @@
         <v>33.6</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,7 +841,7 @@
         <v>1276.8000000000002</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,21 +1022,21 @@
         <v>71</v>
       </c>
       <c r="B24" s="5">
-        <v>100000</v>
+        <v>800000</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B25" s="4">
         <v>0.56000000000000005</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1140,13 +1140,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="4">
         <v>0.08</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1168,29 +1168,29 @@
         <v>109500</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="5">
         <v>200000000</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5">
         <v>800000</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1201,18 +1201,18 @@
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="5">
         <v>1200000</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1251,57 +1251,57 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2">
         <v>0.11853075454128587</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3">
         <v>0.5</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>1.1752104423052856</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5">
         <v>1.5</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1394,13 +1394,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="4">
         <v>0.5</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1439,112 +1439,112 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>0.8</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>0.7</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <v>0.6</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6">
         <v>0.5</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add market to shadow prices correction for all costs.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="125">
   <si>
     <t>turnout_freq</t>
   </si>
@@ -378,6 +378,24 @@
   </si>
   <si>
     <t>Minimum net density to consider a link as being a main track (ton-km/ton = ton).</t>
+  </si>
+  <si>
+    <t>infrast_cost_rpc</t>
+  </si>
+  <si>
+    <t>Shadow price to market price ratio in infrastructure cost (coeff).</t>
+  </si>
+  <si>
+    <t>mobility_cost_rpc</t>
+  </si>
+  <si>
+    <t>Shadow price to market price ratio in mobility cost (coeff).</t>
+  </si>
+  <si>
+    <t>time_cost_rpc</t>
+  </si>
+  <si>
+    <t>Shadow price to market price ratio in time cost (coeff).</t>
   </si>
 </sst>
 </file>
@@ -387,7 +405,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +417,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -424,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -449,6 +474,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,10 +780,10 @@
     <tabColor theme="7" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,6 +1065,17 @@
         <v>115</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0.82</v>
+      </c>
+      <c r="C26" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
@@ -1050,9 +1087,11 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1215,6 +1254,17 @@
         <v>83</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0.82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1225,10 +1275,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,6 +1352,17 @@
       </c>
       <c r="C6" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Repair tests after last changes in cost methods.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -475,6 +475,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1277,7 +1278,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1378,7 +1379,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,8 +1477,8 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,7 +1503,7 @@
       <c r="A2" t="s">
         <v>84</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="11">
         <v>0.8</v>
       </c>
       <c r="C2" t="s">
@@ -1513,7 +1514,7 @@
       <c r="A3" t="s">
         <v>85</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="11">
         <v>0.7</v>
       </c>
       <c r="C3" t="s">
@@ -1524,7 +1525,7 @@
       <c r="A4" t="s">
         <v>86</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="11">
         <v>0.7</v>
       </c>
       <c r="C4" t="s">
@@ -1535,7 +1536,7 @@
       <c r="A5" t="s">
         <v>87</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="11">
         <v>0.6</v>
       </c>
       <c r="C5" t="s">
@@ -1546,7 +1547,7 @@
       <c r="A6" t="s">
         <v>88</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="11">
         <v>0.5</v>
       </c>
       <c r="C6" t="s">

</xml_diff>

<commit_message>
Change derivation maximum coefficients and add new method to cost secondary track.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
   <si>
     <t>turnout_freq</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Design tons for high quality track. Gross tons that a hq track is suposed to support during its lifetime (gross ton-km).</t>
   </si>
   <si>
-    <t>The price of 1km of hight quality track (USD/km).</t>
-  </si>
-  <si>
     <t>max_path_difference</t>
   </si>
   <si>
@@ -396,6 +393,21 @@
   </si>
   <si>
     <t>Shadow price to market price ratio in time cost (coeff).</t>
+  </si>
+  <si>
+    <t>low_quality_track_price</t>
+  </si>
+  <si>
+    <t>The price of 1km of low quality track (USD/km).</t>
+  </si>
+  <si>
+    <t>The price of 1km of high quality track (USD/km).</t>
+  </si>
+  <si>
+    <t>gross_main_min_density</t>
+  </si>
+  <si>
+    <t>Minimum gross density to consider a link as being a main track (ton-km/ton = ton). Used for secondary track eac cost calculation.</t>
   </si>
 </sst>
 </file>
@@ -449,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -476,6 +488,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,7 +797,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +870,7 @@
         <v>33.6</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,7 +881,7 @@
         <v>1276.8000000000002</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1049,32 +1062,32 @@
         <v>71</v>
       </c>
       <c r="B24" s="5">
-        <v>800000</v>
+        <v>100000</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25" s="4">
         <v>0.56000000000000005</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B26" s="10">
         <v>0.82</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1088,10 +1101,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1243,7 @@
         <v>800000</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1241,29 +1254,51 @@
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="5">
         <v>1200000</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B15" s="10">
         <v>0.82</v>
       </c>
       <c r="C15" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="12">
+        <v>200000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="12">
+        <v>1333333.3333333333</v>
+      </c>
+      <c r="C17" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1302,68 +1337,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2">
         <v>0.11853075454128587</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3">
         <v>0.5</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4">
         <v>1.1752104423052856</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B5">
         <v>1.5</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="10">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1379,7 +1414,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,13 +1491,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="4">
         <v>0.5</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1475,10 +1510,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,7 +1523,7 @@
     <col min="3" max="3" width="107.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1499,114 +1534,119 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" s="11">
+        <v>0.875</v>
+      </c>
+      <c r="C3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="11">
-        <v>0.7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4" s="11">
+        <v>0.875</v>
+      </c>
+      <c r="C4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="11">
-        <v>0.7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B5" s="11">
+        <v>0.75</v>
+      </c>
+      <c r="C5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" s="11"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="11">
-        <v>0.6</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6" s="11">
+        <v>0.625</v>
+      </c>
+      <c r="C6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>88</v>
-      </c>
-      <c r="B6" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>89</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add first optimization strategy based on deriving links from one network to the other. Rework many components to support deriving links (as groups of od pairs). Rework deriving methods to allow eventual reversion.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -796,8 +796,8 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +1512,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Rework derivation methods under new and more stable concepts of derivation, that do not depend on the order of derivation scenarios used on one FreightNetwork instance. Infrastructure cost methods still need to be revised under this derivation concept.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -796,7 +796,7 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
@@ -1103,8 +1103,8 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,7 +1284,7 @@
         <v>124</v>
       </c>
       <c r="B16" s="12">
-        <v>200000</v>
+        <v>156250.76923076919</v>
       </c>
       <c r="C16" t="s">
         <v>125</v>
@@ -1295,7 +1295,7 @@
         <v>127</v>
       </c>
       <c r="B17" s="12">
-        <v>1333333.3333333333</v>
+        <v>701400</v>
       </c>
       <c r="C17" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Rework link optimization method and other classes to iterate links sorted by total tons.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -461,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -489,6 +489,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,7 +800,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:C23"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1065,7 @@
         <v>71</v>
       </c>
       <c r="B24" s="5">
-        <v>100000</v>
+        <v>420000</v>
       </c>
       <c r="C24" t="s">
         <v>117</v>
@@ -1083,7 +1086,7 @@
       <c r="A26" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="13">
         <v>0.82</v>
       </c>
       <c r="C26" t="s">

</xml_diff>

<commit_message>
Update gross ton-km methods. Add projection method.
</commit_message>
<xml_diff>
--- a/data/railway_parameters.xlsx
+++ b/data/railway_parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="mobility" sheetId="1" r:id="rId1"/>
@@ -414,8 +414,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -461,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -492,6 +493,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,7 +1108,7 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1515,8 +1517,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,8 +1543,8 @@
       <c r="A2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="11">
-        <v>1</v>
+      <c r="B2" s="14">
+        <v>0.8</v>
       </c>
       <c r="C2" t="s">
         <v>93</v>
@@ -1553,8 +1555,8 @@
       <c r="A3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="11">
-        <v>0.875</v>
+      <c r="B3" s="14">
+        <v>0.7</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
@@ -1565,8 +1567,8 @@
       <c r="A4" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="11">
-        <v>0.875</v>
+      <c r="B4" s="14">
+        <v>0.7</v>
       </c>
       <c r="C4" t="s">
         <v>95</v>
@@ -1577,8 +1579,8 @@
       <c r="A5" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="11">
-        <v>0.75</v>
+      <c r="B5" s="14">
+        <v>0.6</v>
       </c>
       <c r="C5" t="s">
         <v>96</v>
@@ -1589,8 +1591,8 @@
       <c r="A6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="11">
-        <v>0.625</v>
+      <c r="B6" s="14">
+        <v>0.5</v>
       </c>
       <c r="C6" t="s">
         <v>97</v>

</xml_diff>